<commit_message>
LAST PUSH I SWEAR
fixed the issue with Defeat changing to Victory if last enemy reached end with defeat screen open
seriously I'm putting it down now, there cant be anything left to change.
</commit_message>
<xml_diff>
--- a/TSE test cases.xlsx
+++ b/TSE test cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mysticfox99\Downloads\TSE-master(7)\TSE-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\##GITREPOS##\UNI\TSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4BDEEC-8A6D-47D1-880E-8DB57E8FEC91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6D15EB-9D69-400C-9155-CACEB6F771B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{7D06B99A-62CD-46F4-8F1C-E11457077F54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D06B99A-62CD-46F4-8F1C-E11457077F54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>Test cases</t>
   </si>
@@ -122,9 +122,6 @@
   <si>
     <t>Once in editor.
 Once in build.</t>
-  </si>
-  <si>
-    <t>Check tower places correctly</t>
   </si>
   <si>
     <t>1: launch the build, load each individual level once.</t>
@@ -193,10 +190,6 @@
     <t>Win event occurs, allowing return to menu.</t>
   </si>
   <si>
-    <t>Loss event outputs a 
-debug announcing loss.</t>
-  </si>
-  <si>
     <t>Enemy hit has health reduced per shot until destroyed.</t>
   </si>
   <si>
@@ -270,13 +263,40 @@
   </si>
   <si>
     <t>Animations on enemies after implementing an animation controller on enemy scriptable object</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Loss event occurs, allowing return to menu.</t>
+  </si>
+  <si>
+    <t>AE. But if all enemies finish level still grants success</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Not an issue in regular play, but should be investigated.</t>
+  </si>
+  <si>
+    <t>Ruta Greiliha</t>
+  </si>
+  <si>
+    <t>William Smith</t>
+  </si>
+  <si>
+    <t>Towers place correctly</t>
+  </si>
+  <si>
+    <t>Zuzanna Walaszczyk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +337,14 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -389,10 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -412,12 +436,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -441,6 +459,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E079460-F851-4A84-88F3-EF9FEC196CFA}">
-  <dimension ref="B2:J21"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="B2:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,51 +818,59 @@
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="I3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
@@ -825,22 +879,26 @@
         <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="I4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="26">
+        <v>44327</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -854,20 +912,24 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="2:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="I5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="25">
+        <v>44327</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="2:12" ht="36" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -883,18 +945,22 @@
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="G6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="26">
+        <v>44327</v>
+      </c>
+      <c r="K6" s="27"/>
+      <c r="L6" s="24"/>
+    </row>
+    <row r="7" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>4</v>
       </c>
@@ -908,16 +974,26 @@
         <v>19</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="25">
+        <v>44327</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -931,16 +1007,24 @@
         <v>21</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="26">
+        <v>44327</v>
+      </c>
+      <c r="K8" s="27"/>
+      <c r="L8" s="24"/>
+    </row>
+    <row r="9" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>6</v>
       </c>
@@ -948,27 +1032,35 @@
         <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="25">
+        <v>44327</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>25</v>
@@ -977,249 +1069,309 @@
         <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="2:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="26">
+        <v>44328</v>
+      </c>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="2:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="2:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="25">
+        <v>44328</v>
+      </c>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="J12" s="26">
+        <v>44328</v>
+      </c>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="13" t="s">
+      <c r="F13" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="G13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="25">
+        <v>44328</v>
+      </c>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="F14" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="26">
+        <v>44328</v>
+      </c>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="F15" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="25">
+        <v>44328</v>
+      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="26">
+        <v>44328</v>
+      </c>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="2:9" ht="48" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="25">
+        <v>44328</v>
+      </c>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="2:9" ht="72" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="26">
+        <v>44328</v>
+      </c>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
-        <v>17</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="25">
+        <v>44328</v>
+      </c>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="L4:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>